<commit_message>
example for web element screenshot and ocr
</commit_message>
<xml_diff>
--- a/examples/web-stuff/artifact/script/BrowserMeta.xlsx
+++ b/examples/web-stuff/artifact/script/BrowserMeta.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr documentId="13_ncr:1_{4F3F68BE-073B-3D43-B731-6160D64A43C3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="21140" windowWidth="25600" xWindow="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-21140" firstSheet="1"/>
+    <workbookView activeTab="1" firstSheet="1" tabRatio="500" windowHeight="21140" windowWidth="25600" xWindow="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-21140"/>
   </bookViews>
   <sheets>
     <sheet name="#system" r:id="rId1" sheetId="4" state="hidden"/>
@@ -26,9 +26,9 @@
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
-    <definedName name="excel">'#system'!$I$2:$I$14</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$16</definedName>
     <definedName name="external">'#system'!$J$2:$J$6</definedName>
-    <definedName name="image">'#system'!$K$2:$K$7</definedName>
+    <definedName name="image">'#system'!$K$2:$K$8</definedName>
     <definedName name="io">'#system'!$L$2:$L$30</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
@@ -39,7 +39,7 @@
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
     <definedName name="number">'#system'!$R$2:$R$16</definedName>
-    <definedName name="pdf">'#system'!$S$2:$S$16</definedName>
+    <definedName name="pdf">'#system'!$S$2:$S$17</definedName>
     <definedName name="rdbms">'#system'!$T$2:$T$7</definedName>
     <definedName name="redis">'#system'!$U$2:$U$10</definedName>
     <definedName name="sms">'#system'!$V$2:$V$2</definedName>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="594">
   <si>
     <t>description</t>
   </si>
@@ -1849,13 +1849,28 @@
   <si>
     <t>saveAllAsText(var,exclude)</t>
   </si>
+  <si>
+    <t>saveTotalColumnCount(file,worksheet,row,saveVar)</t>
+  </si>
+  <si>
+    <t>saveTotalRowCount(file,worksheet,saveVar)</t>
+  </si>
+  <si>
+    <t>colorbit(image,bit,saveTo)</t>
+  </si>
+  <si>
+    <t>ocr(image,saveVar)</t>
+  </si>
+  <si>
+    <t>saveAsPdf(profile,content,file)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2039,8 +2054,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="31">
+  <fills count="58">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2212,8 +2328,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="67">
     <border>
       <left/>
       <right/>
@@ -2577,6 +2846,332 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -2584,7 +3179,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="69">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -2713,52 +3308,100 @@
     <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="10" fillId="6" fontId="12" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="14" fillId="9" fontId="14" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="18" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="18" fillId="12" fontId="15" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="22" fillId="15" fontId="16" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="18" fontId="18" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="26" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="26" fillId="21" fontId="20" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="30" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="30" fillId="12" fontId="21" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="34" fillId="24" fontId="22" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="34" fillId="24" fontId="23" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="15" fontId="24" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="27" fontId="25" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="15" fontId="26" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="30" fontId="27" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="46" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="39" borderId="50" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="42" borderId="54" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="45" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="48" borderId="58" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="39" borderId="62" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="51" borderId="66" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="51" borderId="66" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="54" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="42" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="57" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3115,7 +3758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF144"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" tabSelected="false">
+    <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -3251,7 +3894,7 @@
         <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>452</v>
+        <v>591</v>
       </c>
       <c r="L2" t="s">
         <v>310</v>
@@ -3583,7 +4226,7 @@
         <v>549</v>
       </c>
       <c r="K6" t="s">
-        <v>343</v>
+        <v>592</v>
       </c>
       <c r="L6" t="s">
         <v>453</v>
@@ -3645,7 +4288,7 @@
         <v>438</v>
       </c>
       <c r="K7" t="s">
-        <v>525</v>
+        <v>343</v>
       </c>
       <c r="L7" t="s">
         <v>70</v>
@@ -3706,6 +4349,9 @@
       <c r="I8" t="s">
         <v>323</v>
       </c>
+      <c r="K8" t="s">
+        <v>525</v>
+      </c>
       <c r="L8" t="s">
         <v>16</v>
       </c>
@@ -3807,7 +4453,7 @@
         <v>301</v>
       </c>
       <c r="I10" t="s">
-        <v>443</v>
+        <v>589</v>
       </c>
       <c r="L10" t="s">
         <v>78</v>
@@ -3851,7 +4497,7 @@
         <v>347</v>
       </c>
       <c r="I11" t="s">
-        <v>317</v>
+        <v>590</v>
       </c>
       <c r="L11" t="s">
         <v>37</v>
@@ -3889,7 +4535,7 @@
         <v>269</v>
       </c>
       <c r="I12" t="s">
-        <v>318</v>
+        <v>443</v>
       </c>
       <c r="L12" t="s">
         <v>477</v>
@@ -3927,7 +4573,7 @@
         <v>258</v>
       </c>
       <c r="I13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L13" t="s">
         <v>381</v>
@@ -3939,7 +4585,7 @@
         <v>92</v>
       </c>
       <c r="S13" t="s">
-        <v>250</v>
+        <v>593</v>
       </c>
       <c r="Z13" t="s">
         <v>321</v>
@@ -3962,7 +4608,7 @@
         <v>311</v>
       </c>
       <c r="I14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L14" t="s">
         <v>17</v>
@@ -3974,7 +4620,7 @@
         <v>93</v>
       </c>
       <c r="S14" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="Z14" t="s">
         <v>100</v>
@@ -3996,6 +4642,9 @@
       <c r="H15" t="s">
         <v>259</v>
       </c>
+      <c r="I15" t="s">
+        <v>319</v>
+      </c>
       <c r="L15" t="s">
         <v>41</v>
       </c>
@@ -4006,7 +4655,7 @@
         <v>482</v>
       </c>
       <c r="S15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Z15" t="s">
         <v>581</v>
@@ -4028,6 +4677,9 @@
       <c r="H16" t="s">
         <v>260</v>
       </c>
+      <c r="I16" t="s">
+        <v>320</v>
+      </c>
       <c r="L16" t="s">
         <v>478</v>
       </c>
@@ -4038,7 +4690,7 @@
         <v>483</v>
       </c>
       <c r="S16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Z16" t="s">
         <v>101</v>
@@ -4065,6 +4717,9 @@
       </c>
       <c r="N17" t="s">
         <v>39</v>
+      </c>
+      <c r="S17" t="s">
+        <v>248</v>
       </c>
       <c r="Z17" t="s">
         <v>73</v>

</xml_diff>